<commit_message>
Refactor: Updated Combat Mastery Unit tests to be consistent with new Character constructor
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/BlackBox_Character.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/BlackBox_Character.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\Character\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1253F9-34C3-482E-87E9-D3CC7DE0DD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB391AD0-604D-4133-ABFC-3C287C83D8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
   </bookViews>
   <sheets>
     <sheet name="Constructor" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="44">
   <si>
     <t>Test Case</t>
   </si>
@@ -64,18 +64,9 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Level = 1</t>
-  </si>
-  <si>
     <t>Valid Input</t>
   </si>
   <si>
-    <t>Level = 2</t>
-  </si>
-  <si>
-    <t>Level = 5</t>
-  </si>
-  <si>
     <t>Low even number</t>
   </si>
   <si>
@@ -88,15 +79,6 @@
     <t>High even number</t>
   </si>
   <si>
-    <t>Level = 12</t>
-  </si>
-  <si>
-    <t>Level = 17</t>
-  </si>
-  <si>
-    <t>Level = 20</t>
-  </si>
-  <si>
     <t>High odd number</t>
   </si>
   <si>
@@ -176,6 +158,24 @@
   </si>
   <si>
     <t>Bard</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>ancestry</t>
+  </si>
+  <si>
+    <t>might</t>
+  </si>
+  <si>
+    <t>agility</t>
+  </si>
+  <si>
+    <t>charisma</t>
+  </si>
+  <si>
+    <t>intelligence</t>
   </si>
 </sst>
 </file>
@@ -227,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -241,11 +241,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,38 +602,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -648,10 +651,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8D1AFC-88D1-4A6F-9560-98E936705A52}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,13 +662,18 @@
     <col min="1" max="1" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,122 +683,259 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="7">
+        <v>3</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>2</v>
+      </c>
+      <c r="J3" s="7">
+        <v>-2</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2</v>
+      </c>
+      <c r="J4" s="7">
+        <v>-2</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="7">
+        <v>3</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>2</v>
+      </c>
+      <c r="J5" s="7">
+        <v>-2</v>
+      </c>
+      <c r="K5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>-2</v>
+      </c>
+      <c r="K6" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="7">
+        <v>3</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2</v>
+      </c>
+      <c r="J7" s="7">
+        <v>-2</v>
+      </c>
+      <c r="K7" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="7">
+        <v>3</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2</v>
+      </c>
+      <c r="J8" s="7">
+        <v>-2</v>
+      </c>
+      <c r="K8" s="7">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -843,10 +988,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -860,10 +1005,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3" s="4">
         <v>3</v>
@@ -877,10 +1022,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4">
         <v>5</v>
@@ -894,10 +1039,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4">
         <v>7</v>
@@ -911,10 +1056,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4">
         <v>10</v>
@@ -928,10 +1073,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D7" s="4">
         <v>13</v>
@@ -945,10 +1090,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4">
         <v>15</v>
@@ -962,10 +1107,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4">
         <v>18</v>
@@ -979,10 +1124,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10" s="4">
         <v>20</v>
@@ -1020,60 +1165,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1099,10 +1244,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1128,10 +1273,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1157,10 +1302,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -1186,10 +1331,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -1227,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB43AFB8-132D-4E2B-BACC-B0D3E98F4493}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,68 +1393,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1327,16 +1472,16 @@
         <v>-2</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K3" s="4">
         <v>11</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>39</v>
+      <c r="L3" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1344,10 +1489,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1365,25 +1510,25 @@
         <v>-2</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K4" s="4">
         <v>11</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1401,10 +1546,10 @@
         <v>-2</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K5" s="4">
         <v>10</v>
@@ -1434,67 +1579,67 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1524,67 +1669,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1614,67 +1759,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1704,67 +1849,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor: Updated Prime Attribute Units tests and character constructor to match update.
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/BlackBox_Character.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/BlackBox_Character.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB391AD0-604D-4133-ABFC-3C287C83D8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC6DB8-DF4F-49A6-9C64-69C83D1F30BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
   </bookViews>
   <sheets>
     <sheet name="Constructor" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="44">
   <si>
     <t>Test Case</t>
   </si>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8D1AFC-88D1-4A6F-9560-98E936705A52}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,10 +1143,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B60139-BDA5-4694-95B4-B5CCD376AFD6}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,16 +1155,18 @@
     <col min="2" max="2" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="5" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1181,14 +1183,16 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1196,21 +1200,27 @@
         <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1223,23 +1233,29 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="4">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
+      <c r="E3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="G3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
         <v>-2</v>
       </c>
-      <c r="I3" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1252,23 +1268,29 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="4">
         <v>-2</v>
       </c>
-      <c r="F4" s="4">
-        <v>3</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
       <c r="H4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>2</v>
+      </c>
+      <c r="K4" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1281,23 +1303,29 @@
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="4">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
         <v>-2</v>
       </c>
-      <c r="G5" s="4">
-        <v>3</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
       <c r="I5" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1310,23 +1338,29 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
-        <v>2</v>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4">
         <v>-2</v>
       </c>
-      <c r="H6" s="4">
-        <v>3</v>
-      </c>
-      <c r="I6" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="4">
+        <v>3</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1339,28 +1373,34 @@
       <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="4">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4">
-        <v>3</v>
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="G7" s="4">
+        <v>3</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3</v>
+      </c>
+      <c r="I7" s="4">
         <v>0</v>
       </c>
-      <c r="H7" s="4">
+      <c r="J7" s="4">
         <v>-2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="K7" s="4">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>

</xml_diff>

<commit_message>
Test: Update unit test spreadsheet to be in line with coded unit tests
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/BlackBox_Character.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/BlackBox_Character.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC6DB8-DF4F-49A6-9C64-69C83D1F30BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2763FEB-4547-482E-A663-4E0E90FB40FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="4" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
   </bookViews>
   <sheets>
     <sheet name="Constructor" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="48">
   <si>
     <t>Test Case</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Barbarian</t>
   </si>
   <si>
-    <t>Bard</t>
-  </si>
-  <si>
     <t>class</t>
   </si>
   <si>
@@ -176,6 +173,21 @@
   </si>
   <si>
     <t>intelligence</t>
+  </si>
+  <si>
+    <t>mightSave</t>
+  </si>
+  <si>
+    <t>agilitySave</t>
+  </si>
+  <si>
+    <t>charsimaSave</t>
+  </si>
+  <si>
+    <t>intelligenceSave</t>
+  </si>
+  <si>
+    <t>Barbarian, higher level</t>
   </si>
 </sst>
 </file>
@@ -651,10 +663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8D1AFC-88D1-4A6F-9560-98E936705A52}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D2" sqref="D2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,15 +677,20 @@
     <col min="4" max="4" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,37 +709,53 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -744,20 +777,32 @@
       <c r="G3" s="7">
         <v>3</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I3" s="7">
-        <v>2</v>
-      </c>
-      <c r="J3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="7">
+        <v>2</v>
+      </c>
+      <c r="L3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
         <v>-2</v>
       </c>
-      <c r="K3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -779,20 +824,32 @@
       <c r="G4" s="7">
         <v>3</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I4" s="7">
-        <v>2</v>
-      </c>
-      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
         <v>-2</v>
       </c>
-      <c r="K4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -814,20 +871,32 @@
       <c r="G5" s="7">
         <v>3</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="7">
-        <v>2</v>
-      </c>
-      <c r="J5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
         <v>-2</v>
       </c>
-      <c r="K5" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -849,20 +918,32 @@
       <c r="G6" s="7">
         <v>3</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I6" s="7">
-        <v>2</v>
-      </c>
-      <c r="J6" s="7">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
         <v>-2</v>
       </c>
-      <c r="K6" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -884,20 +965,32 @@
       <c r="G7" s="7">
         <v>3</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I7" s="7">
-        <v>2</v>
-      </c>
-      <c r="J7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
         <v>-2</v>
       </c>
-      <c r="K7" s="7">
+      <c r="N7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -919,22 +1012,34 @@
       <c r="G8" s="7">
         <v>3</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I8" s="7">
-        <v>2</v>
-      </c>
-      <c r="J8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
         <v>-2</v>
       </c>
-      <c r="K8" s="7">
+      <c r="N8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="D1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1143,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B60139-BDA5-4694-95B4-B5CCD376AFD6}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,17 +1261,23 @@
     <col min="3" max="3" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="4"/>
+    <col min="6" max="6" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1185,14 +1296,18 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1200,27 +1315,39 @@
         <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1242,20 +1369,32 @@
       <c r="G3" s="4">
         <v>3</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="I3" s="4">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>2</v>
+      </c>
+      <c r="L3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
         <v>-2</v>
       </c>
-      <c r="K3" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1277,20 +1416,32 @@
       <c r="G4" s="4">
         <v>-2</v>
       </c>
-      <c r="H4" s="4">
-        <v>3</v>
+      <c r="H4" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="J4" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="K4" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1312,20 +1463,32 @@
       <c r="G5" s="4">
         <v>2</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
         <v>-2</v>
       </c>
-      <c r="I5" s="4">
-        <v>3</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="J5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="K5" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1347,20 +1510,32 @@
       <c r="G6" s="4">
         <v>1</v>
       </c>
-      <c r="H6" s="4">
-        <v>2</v>
+      <c r="H6" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="I6" s="4">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
         <v>-2</v>
       </c>
-      <c r="J6" s="4">
-        <v>3</v>
-      </c>
-      <c r="K6" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>3</v>
+      </c>
+      <c r="N6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1382,27 +1557,39 @@
       <c r="G7" s="4">
         <v>3</v>
       </c>
-      <c r="H7" s="4">
-        <v>3</v>
+      <c r="H7" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
+        <v>3</v>
+      </c>
+      <c r="J7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
         <v>-2</v>
       </c>
-      <c r="K7" s="4">
+      <c r="N7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1410,29 +1597,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB43AFB8-132D-4E2B-BACC-B0D3E98F4493}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1451,14 +1642,18 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1466,27 +1661,39 @@
         <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1494,115 +1701,117 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="G3" s="4">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>2</v>
+      </c>
+      <c r="L3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
         <v>-2</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="N3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>11</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="4">
-        <v>11</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
       <c r="G4" s="4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
         <v>-2</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="4">
-        <v>11</v>
-      </c>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>-2</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="4">
-        <v>10</v>
-      </c>
+      <c r="N4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>13</v>
+      </c>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="D1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>